<commit_message>
Update with updates for presentation
</commit_message>
<xml_diff>
--- a/Relatorio_Tempos_de_execucao_Ordenacao.xlsx
+++ b/Relatorio_Tempos_de_execucao_Ordenacao.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ADS_2021\Analise e Estrutura de Dados\Trabalho Ordenação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E2C5AD-B56B-4EB8-ABFB-1F01D8115582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB575AF-AC7E-4B8C-A3CB-0D1912F83AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2850" windowWidth="29040" windowHeight="15840" xr2:uid="{AC139EAF-251F-4372-ABA3-0D40D21E2EB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AC139EAF-251F-4372-ABA3-0D40D21E2EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Bubble Sort</t>
   </si>
@@ -66,6 +67,33 @@
   </si>
   <si>
     <t>Gabriel de Castro</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>50K</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>150K</t>
+  </si>
+  <si>
+    <t>200K</t>
+  </si>
+  <si>
+    <t>300K</t>
+  </si>
+  <si>
+    <t>400K</t>
+  </si>
+  <si>
+    <t>519K</t>
+  </si>
+  <si>
+    <t>500K</t>
   </si>
 </sst>
 </file>
@@ -108,10 +136,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1663,6 +1691,946 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.064</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.723999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.352000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>147.75200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>263.18400000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>393.28300000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8810000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.736000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.956</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>114.553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>308.54000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.522</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45.540999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103.31399999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>203.131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>285.38400000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heap Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Planilha2!$C$2:$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5K</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50K</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100K</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150K</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200K</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300K</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400K</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$C$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E6AB-4D62-8527-E2CA47922FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="492628607"/>
+        <c:axId val="492625695"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="492628607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492625695"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="492625695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492628607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1743,6 +2711,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -2731,6 +3739,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2804,6 +4328,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02685CD6-448C-623F-3CB1-14C18FF28AF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3111,8 +4676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7593501B-B6A0-44B0-8570-65DE8BF2081A}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3128,15 +4693,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -3296,25 +4861,25 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>44.74</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>7.75</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>14.92</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2.7E-2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>1.2E-2</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>1.6E-2</v>
       </c>
     </row>
@@ -3322,25 +4887,25 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>25.01</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>6.84</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>12.22</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>3.1E-2</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
@@ -3353,13 +4918,280 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED85A52-B4A4-46EE-8B08-AC8F639CD932}">
+  <dimension ref="B2:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J9" sqref="B2:J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>3.9849999999999999</v>
+      </c>
+      <c r="E3">
+        <v>24.064</v>
+      </c>
+      <c r="F3">
+        <v>47.723999999999997</v>
+      </c>
+      <c r="G3">
+        <v>72.352000000000004</v>
+      </c>
+      <c r="H3">
+        <v>147.75200000000001</v>
+      </c>
+      <c r="I3">
+        <v>263.18400000000003</v>
+      </c>
+      <c r="J3">
+        <v>393.28300000000002</v>
+      </c>
+      <c r="K3">
+        <v>387.03899999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.6140000000000001</v>
+      </c>
+      <c r="E4">
+        <v>9.8810000000000002</v>
+      </c>
+      <c r="F4">
+        <v>26.994</v>
+      </c>
+      <c r="G4">
+        <v>25.736000000000001</v>
+      </c>
+      <c r="H4">
+        <v>105.956</v>
+      </c>
+      <c r="I4">
+        <v>114.553</v>
+      </c>
+      <c r="J4">
+        <v>308.54000000000002</v>
+      </c>
+      <c r="K4">
+        <v>224.91399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.8940000000000001</v>
+      </c>
+      <c r="E5">
+        <v>11.522</v>
+      </c>
+      <c r="F5">
+        <v>25.593</v>
+      </c>
+      <c r="G5">
+        <v>45.540999999999997</v>
+      </c>
+      <c r="H5">
+        <v>103.31399999999999</v>
+      </c>
+      <c r="I5">
+        <v>203.131</v>
+      </c>
+      <c r="J5">
+        <v>285.38400000000001</v>
+      </c>
+      <c r="K5">
+        <v>307.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.01</v>
+      </c>
+      <c r="E6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.06</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="J6">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G7">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I7">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="K7">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F8">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>3.1E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.06</v>
+      </c>
+      <c r="I8">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="K8">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F9">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H9">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="J9">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E2EAA744F8B4BF44BAC78B85DDB8A9CB" ma:contentTypeVersion="5" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="b10593423ac5f22e7150ae05066c5fad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ed7ca3f1-ef3a-48ed-ad19-a8764e60fd66" xmlns:ns4="18fb6223-781c-4cd9-b0b6-0ffde7a12554" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2e8c4d107a2568900e80f025dc93d87" ns3:_="" ns4:_="">
     <xsd:import namespace="ed7ca3f1-ef3a-48ed-ad19-a8764e60fd66"/>
@@ -3530,7 +5362,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3539,24 +5371,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC115AC-4548-4C50-A527-A64D17DB4817}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18fb6223-781c-4cd9-b0b6-0ffde7a12554"/>
-    <ds:schemaRef ds:uri="ed7ca3f1-ef3a-48ed-ad19-a8764e60fd66"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0254E3B7-0F9E-4EF4-9C2E-1FACF04CD278}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3575,10 +5396,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5943723A-BDA1-49C6-A13D-5983444A44B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC115AC-4548-4C50-A527-A64D17DB4817}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18fb6223-781c-4cd9-b0b6-0ffde7a12554"/>
+    <ds:schemaRef ds:uri="ed7ca3f1-ef3a-48ed-ad19-a8764e60fd66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>